<commit_message>
Adjusted some of the PCS Aggregation calcs
now avoids nulls, normalises to range(0,1) for Risk and Poverty
</commit_message>
<xml_diff>
--- a/PCS/dashboard.xlsx
+++ b/PCS/dashboard.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9492" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9492" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
-    <sheet name="DASH_MIRROR" sheetId="3" r:id="rId2"/>
-    <sheet name="ROUGHNESS" sheetId="5" state="hidden" r:id="rId3"/>
-    <sheet name="HAZARD" sheetId="4" r:id="rId4"/>
+    <sheet name="DASH_MIRROR" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="ROUGHNESS" sheetId="5" r:id="rId3"/>
+    <sheet name="HAZARD" sheetId="4" state="hidden" r:id="rId4"/>
     <sheet name="POV" sheetId="7" state="hidden" r:id="rId5"/>
-    <sheet name="CRITICALITY" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="CRITICALITY" sheetId="6" r:id="rId6"/>
     <sheet name="Ref" sheetId="2" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -162,6 +162,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="C60" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Charles Fox:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ensure shapefile in criticality input folder is the same name as the name written here</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D60" authorId="0" shapeId="0">
       <text>
         <r>
@@ -183,6 +207,30 @@
           </rPr>
           <t xml:space="preserve">
 column in the input shapefile that describes the relative attractiveness / business of each node. E.g. for admin boundaries, 'population' ought to be used, and for hospitals, an indicator of the size or regional importance of the hospital, e.g. 'number of beds'.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C66" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Charles Fox:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ensure shapefile in criticality input folder is the same name as the name written here</t>
         </r>
       </text>
     </comment>
@@ -283,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E74" authorId="0" shapeId="0">
+    <comment ref="E82" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -307,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C81" authorId="0" shapeId="0">
+    <comment ref="C89" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -331,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C82" authorId="0" shapeId="0">
+    <comment ref="C90" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -360,7 +408,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="259">
   <si>
     <t>Proportion of people living in a house with solid roof</t>
   </si>
@@ -1013,9 +1061,6 @@
     <t>IRI Score =  (</t>
   </si>
   <si>
-    <t>Standard deviation of IRI</t>
-  </si>
-  <si>
     <t xml:space="preserve">Minimum IRI </t>
   </si>
   <si>
@@ -1055,9 +1100,6 @@
     <t>iri_max</t>
   </si>
   <si>
-    <t>iri_stdev</t>
-  </si>
-  <si>
     <t>iri_mean</t>
   </si>
   <si>
@@ -1122,6 +1164,27 @@
   </si>
   <si>
     <t>Component</t>
+  </si>
+  <si>
+    <t>Combinations</t>
+  </si>
+  <si>
+    <t>Combination number</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>ComboNumber</t>
+  </si>
+  <si>
+    <t>ComboO</t>
+  </si>
+  <si>
+    <t>ComboD</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1197,7 @@
     <numFmt numFmtId="166" formatCode="#,###\ &quot;Degrees Centigrade&quot;"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1209,13 +1272,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -1264,6 +1320,41 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="19">
@@ -1961,9 +2052,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2056,16 +2147,6 @@
     <xf numFmtId="9" fontId="9" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2081,8 +2162,8 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2113,9 +2194,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -2152,7 +2230,6 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2170,11 +2247,32 @@
     <xf numFmtId="9" fontId="1" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="15" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="14" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3717,10 +3815,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:O84"/>
+  <dimension ref="A1:O92"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView showGridLines="0" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L79" sqref="L79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3831,7 +3929,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="43"/>
-      <c r="C7" s="59"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3847,7 +3945,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" s="43"/>
-      <c r="C8" s="60"/>
+      <c r="C8" s="56"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -3895,9 +3993,9 @@
       <c r="H10" s="44"/>
       <c r="J10" s="23"/>
       <c r="K10" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="L10" s="65"/>
+        <v>221</v>
+      </c>
+      <c r="L10" s="61"/>
       <c r="M10" s="35">
         <v>0.2</v>
       </c>
@@ -3917,9 +4015,9 @@
       <c r="H11" s="44"/>
       <c r="J11" s="23"/>
       <c r="K11" s="23" t="s">
-        <v>223</v>
-      </c>
-      <c r="L11" s="65"/>
+        <v>222</v>
+      </c>
+      <c r="L11" s="61"/>
       <c r="M11" s="35">
         <v>0.2</v>
       </c>
@@ -3939,9 +4037,9 @@
       <c r="H12" s="44"/>
       <c r="J12" s="23"/>
       <c r="K12" s="23" t="s">
-        <v>224</v>
-      </c>
-      <c r="L12" s="65"/>
+        <v>223</v>
+      </c>
+      <c r="L12" s="61"/>
       <c r="M12" s="35">
         <v>0.25</v>
       </c>
@@ -3961,9 +4059,9 @@
       <c r="H13" s="44"/>
       <c r="J13" s="23"/>
       <c r="K13" s="23" t="s">
-        <v>225</v>
-      </c>
-      <c r="L13" s="65"/>
+        <v>224</v>
+      </c>
+      <c r="L13" s="61"/>
       <c r="M13" s="35">
         <v>0.25</v>
       </c>
@@ -3983,9 +4081,9 @@
       <c r="H14" s="44"/>
       <c r="J14" s="23"/>
       <c r="K14" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="L14" s="65"/>
+        <v>225</v>
+      </c>
+      <c r="L14" s="61"/>
       <c r="M14" s="35">
         <v>0.1</v>
       </c>
@@ -4091,7 +4189,7 @@
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="45"/>
-      <c r="C20" s="55" t="str">
+      <c r="C20" s="51" t="str">
         <f>IF(D20=1,"OK","ERROR! Ensure Weighting total = 100%")</f>
         <v>OK</v>
       </c>
@@ -4353,7 +4451,7 @@
       <c r="E36" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F36" s="54">
+      <c r="F36" s="50">
         <v>50</v>
       </c>
       <c r="G36" s="12"/>
@@ -4375,7 +4473,7 @@
       <c r="E37" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F37" s="54">
+      <c r="F37" s="50">
         <v>50</v>
       </c>
       <c r="G37" s="12"/>
@@ -4397,7 +4495,7 @@
       <c r="E38" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F38" s="58">
+      <c r="F38" s="54">
         <v>0.5</v>
       </c>
       <c r="G38" s="12"/>
@@ -4419,7 +4517,7 @@
       <c r="E39" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F39" s="58">
+      <c r="F39" s="54">
         <v>0.5</v>
       </c>
       <c r="G39" s="12"/>
@@ -4441,7 +4539,7 @@
       <c r="E40" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F40" s="58">
+      <c r="F40" s="54">
         <v>0.5</v>
       </c>
       <c r="G40" s="12"/>
@@ -4463,7 +4561,7 @@
       <c r="E41" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F41" s="58">
+      <c r="F41" s="54">
         <v>0.5</v>
       </c>
       <c r="G41" s="12"/>
@@ -4485,7 +4583,7 @@
       <c r="E42" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F42" s="58">
+      <c r="F42" s="54">
         <v>0.5</v>
       </c>
       <c r="G42" s="12"/>
@@ -4507,7 +4605,7 @@
       <c r="E43" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="58">
+      <c r="F43" s="54">
         <v>0.5</v>
       </c>
       <c r="G43" s="12"/>
@@ -4529,7 +4627,7 @@
       <c r="E44" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F44" s="58">
+      <c r="F44" s="54">
         <v>0.5</v>
       </c>
       <c r="G44" s="12"/>
@@ -4551,7 +4649,7 @@
       <c r="E45" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F45" s="58">
+      <c r="F45" s="54">
         <v>0.5</v>
       </c>
       <c r="G45" s="12"/>
@@ -4573,7 +4671,7 @@
       <c r="E46" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F46" s="58">
+      <c r="F46" s="54">
         <v>0.5</v>
       </c>
       <c r="G46" s="12"/>
@@ -4595,7 +4693,7 @@
       <c r="E47" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F47" s="64">
+      <c r="F47" s="60">
         <v>30</v>
       </c>
       <c r="G47" s="12"/>
@@ -4617,7 +4715,7 @@
       <c r="E48" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F48" s="64">
+      <c r="F48" s="60">
         <v>30</v>
       </c>
       <c r="G48" s="12"/>
@@ -4639,7 +4737,7 @@
       <c r="E49" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F49" s="64">
+      <c r="F49" s="60">
         <v>30</v>
       </c>
       <c r="G49" s="12"/>
@@ -4752,11 +4850,11 @@
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B55" s="14"/>
-      <c r="C55" s="56" t="str">
+      <c r="C55" s="52" t="str">
         <f>IF(D55=1,"OK","ERROR! Ensure Weighting total = 100%")</f>
         <v>OK</v>
       </c>
-      <c r="D55" s="57">
+      <c r="D55" s="53">
         <f>SUM(D36:D54)</f>
         <v>1.0000000000000002</v>
       </c>
@@ -4771,75 +4869,75 @@
       <c r="N55" s="28"/>
     </row>
     <row r="57" spans="2:14" ht="21" x14ac:dyDescent="0.4">
-      <c r="B57" s="71" t="s">
+      <c r="B57" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C57" s="72"/>
-      <c r="D57" s="73"/>
-      <c r="E57" s="73"/>
-      <c r="F57" s="73"/>
-      <c r="G57" s="73"/>
-      <c r="H57" s="74"/>
-      <c r="J57" s="87" t="s">
+      <c r="C57" s="68"/>
+      <c r="D57" s="69"/>
+      <c r="E57" s="69"/>
+      <c r="F57" s="69"/>
+      <c r="G57" s="69"/>
+      <c r="H57" s="70"/>
+      <c r="J57" s="82" t="s">
         <v>213</v>
       </c>
-      <c r="K57" s="88"/>
-      <c r="L57" s="88"/>
-      <c r="M57" s="88"/>
-      <c r="N57" s="89"/>
+      <c r="K57" s="83"/>
+      <c r="L57" s="83"/>
+      <c r="M57" s="83"/>
+      <c r="N57" s="84"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B58" s="66"/>
+      <c r="B58" s="62"/>
       <c r="C58" s="24"/>
       <c r="D58" s="24"/>
       <c r="E58" s="24"/>
       <c r="F58" s="24"/>
       <c r="G58" s="24"/>
-      <c r="H58" s="67"/>
-      <c r="J58" s="93"/>
-      <c r="K58" s="94"/>
-      <c r="L58" s="94"/>
-      <c r="M58" s="94"/>
-      <c r="N58" s="95"/>
+      <c r="H58" s="63"/>
+      <c r="J58" s="88"/>
+      <c r="K58" s="89"/>
+      <c r="L58" s="89"/>
+      <c r="M58" s="89"/>
+      <c r="N58" s="90"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B59" s="66"/>
-      <c r="C59" s="80" t="s">
+      <c r="B59" s="62"/>
+      <c r="C59" s="116" t="s">
         <v>194</v>
       </c>
-      <c r="D59" s="81"/>
+      <c r="D59" s="76"/>
       <c r="E59" s="24"/>
       <c r="F59" s="24"/>
       <c r="G59" s="24"/>
-      <c r="H59" s="67"/>
-      <c r="J59" s="93"/>
-      <c r="K59" s="94" t="s">
+      <c r="H59" s="63"/>
+      <c r="J59" s="88"/>
+      <c r="K59" s="89" t="s">
         <v>214</v>
       </c>
-      <c r="L59" s="94"/>
-      <c r="M59" s="94"/>
-      <c r="N59" s="95"/>
+      <c r="L59" s="89"/>
+      <c r="M59" s="89"/>
+      <c r="N59" s="90"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B60" s="66"/>
-      <c r="C60" s="76" t="s">
+      <c r="B60" s="62"/>
+      <c r="C60" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="D60" s="79" t="s">
+      <c r="D60" s="75" t="s">
         <v>197</v>
       </c>
       <c r="E60" s="24"/>
       <c r="F60" s="24"/>
       <c r="G60" s="24"/>
-      <c r="H60" s="67"/>
-      <c r="J60" s="93"/>
-      <c r="K60" s="94"/>
-      <c r="L60" s="94"/>
-      <c r="M60" s="94"/>
-      <c r="N60" s="95"/>
+      <c r="H60" s="63"/>
+      <c r="J60" s="88"/>
+      <c r="K60" s="89"/>
+      <c r="L60" s="89"/>
+      <c r="M60" s="89"/>
+      <c r="N60" s="90"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B61" s="66"/>
+      <c r="B61" s="62"/>
       <c r="C61" s="8" t="s">
         <v>200</v>
       </c>
@@ -4849,453 +4947,586 @@
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
       <c r="G61" s="24"/>
-      <c r="H61" s="67"/>
-      <c r="J61" s="93"/>
-      <c r="K61" s="94" t="s">
-        <v>221</v>
-      </c>
-      <c r="L61" s="94"/>
-      <c r="M61" s="94"/>
-      <c r="N61" s="95"/>
+      <c r="H61" s="63"/>
+      <c r="J61" s="88"/>
+      <c r="K61" s="89" t="s">
+        <v>220</v>
+      </c>
+      <c r="L61" s="89"/>
+      <c r="M61" s="89"/>
+      <c r="N61" s="90"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B62" s="66"/>
+      <c r="B62" s="62"/>
       <c r="C62" s="8"/>
       <c r="D62" s="2"/>
       <c r="E62" s="24"/>
       <c r="F62" s="24"/>
       <c r="G62" s="24"/>
-      <c r="H62" s="67"/>
-      <c r="J62" s="93"/>
-      <c r="K62" s="94"/>
-      <c r="L62" s="94"/>
-      <c r="M62" s="94"/>
-      <c r="N62" s="95"/>
+      <c r="H62" s="63"/>
+      <c r="J62" s="88"/>
+      <c r="K62" s="89"/>
+      <c r="L62" s="89"/>
+      <c r="M62" s="89"/>
+      <c r="N62" s="90"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B63" s="66"/>
+      <c r="B63" s="62"/>
       <c r="C63" s="8"/>
       <c r="D63" s="2"/>
       <c r="E63" s="24"/>
       <c r="F63" s="24"/>
       <c r="G63" s="24"/>
-      <c r="H63" s="67"/>
-      <c r="J63" s="93"/>
-      <c r="K63" s="90" t="s">
+      <c r="H63" s="63"/>
+      <c r="J63" s="88"/>
+      <c r="K63" s="85" t="s">
         <v>206</v>
       </c>
-      <c r="L63" s="91"/>
-      <c r="M63" s="90" t="s">
+      <c r="L63" s="86"/>
+      <c r="M63" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="N63" s="95"/>
+      <c r="N63" s="90"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B64" s="66"/>
+      <c r="B64" s="62"/>
       <c r="C64" s="24"/>
       <c r="D64" s="24"/>
-      <c r="E64" s="78"/>
-      <c r="F64" s="78"/>
-      <c r="G64" s="78"/>
-      <c r="H64" s="67"/>
-      <c r="J64" s="93"/>
-      <c r="K64" s="92" t="s">
+      <c r="E64" s="74"/>
+      <c r="F64" s="74"/>
+      <c r="G64" s="74"/>
+      <c r="H64" s="63"/>
+      <c r="J64" s="88"/>
+      <c r="K64" s="87" t="s">
         <v>215</v>
       </c>
-      <c r="L64" s="77"/>
+      <c r="L64" s="73"/>
       <c r="M64" s="2">
         <v>0.6</v>
       </c>
-      <c r="N64" s="95"/>
+      <c r="N64" s="90"/>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B65" s="66"/>
-      <c r="C65" s="80" t="s">
+      <c r="B65" s="62"/>
+      <c r="C65" s="116" t="s">
         <v>195</v>
       </c>
-      <c r="D65" s="81"/>
-      <c r="E65" s="81"/>
-      <c r="F65" s="81"/>
-      <c r="G65" s="81"/>
-      <c r="H65" s="67"/>
-      <c r="J65" s="93"/>
-      <c r="K65" s="92" t="s">
+      <c r="D65" s="76"/>
+      <c r="E65" s="76"/>
+      <c r="F65" s="76"/>
+      <c r="G65" s="76"/>
+      <c r="H65" s="63"/>
+      <c r="J65" s="88"/>
+      <c r="K65" s="87" t="s">
         <v>217</v>
       </c>
-      <c r="L65" s="77"/>
+      <c r="L65" s="73"/>
       <c r="M65" s="2">
         <v>0.1</v>
       </c>
-      <c r="N65" s="95"/>
+      <c r="N65" s="90"/>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B66" s="66"/>
-      <c r="C66" s="76" t="s">
+      <c r="B66" s="62"/>
+      <c r="C66" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="D66" s="79" t="s">
+      <c r="D66" s="75" t="s">
         <v>197</v>
       </c>
-      <c r="E66" s="79" t="s">
+      <c r="E66" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="F66" s="79" t="s">
+      <c r="F66" s="75" t="s">
         <v>199</v>
       </c>
-      <c r="G66" s="79" t="s">
-        <v>251</v>
-      </c>
-      <c r="H66" s="67"/>
-      <c r="J66" s="93"/>
-      <c r="K66" s="92" t="s">
+      <c r="G66" s="75" t="s">
+        <v>249</v>
+      </c>
+      <c r="H66" s="63"/>
+      <c r="J66" s="88"/>
+      <c r="K66" s="87" t="s">
         <v>218</v>
       </c>
-      <c r="L66" s="77"/>
+      <c r="L66" s="73"/>
       <c r="M66" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="N66" s="95"/>
+        <v>0.2</v>
+      </c>
+      <c r="N66" s="90"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B67" s="66"/>
+      <c r="B67" s="62"/>
       <c r="C67" s="8" t="s">
         <v>200</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E67" s="115">
+      <c r="E67" s="109">
         <v>1000</v>
       </c>
-      <c r="F67" s="77">
+      <c r="F67" s="73">
         <v>50</v>
       </c>
-      <c r="G67" s="77">
+      <c r="G67" s="73">
         <v>1</v>
       </c>
-      <c r="H67" s="67"/>
-      <c r="J67" s="93"/>
-      <c r="K67" s="92" t="s">
+      <c r="H67" s="63"/>
+      <c r="J67" s="88"/>
+      <c r="K67" s="87" t="s">
         <v>219</v>
       </c>
-      <c r="L67" s="77"/>
+      <c r="L67" s="73"/>
       <c r="M67" s="2">
         <v>0.1</v>
       </c>
-      <c r="N67" s="95"/>
+      <c r="N67" s="90"/>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B68" s="66"/>
+      <c r="B68" s="62"/>
       <c r="C68" s="8" t="s">
         <v>203</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E68" s="115">
+      <c r="E68" s="109">
         <v>10000</v>
       </c>
-      <c r="F68" s="77">
+      <c r="F68" s="73">
         <v>3</v>
       </c>
-      <c r="G68" s="77">
+      <c r="G68" s="73">
         <v>5</v>
       </c>
-      <c r="H68" s="67"/>
-      <c r="J68" s="93"/>
-      <c r="K68" s="92" t="s">
-        <v>220</v>
-      </c>
-      <c r="L68" s="77"/>
-      <c r="M68" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="N68" s="95"/>
+      <c r="H68" s="63"/>
+      <c r="J68" s="88"/>
+      <c r="K68" s="94" t="str">
+        <f>IF(M68=1,"OK","ERROR! Ensure Weighting total = 100%")</f>
+        <v>OK</v>
+      </c>
+      <c r="L68" s="89"/>
+      <c r="M68" s="97">
+        <f>SUM(M64:M67)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="N68" s="90"/>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B69" s="66"/>
+      <c r="B69" s="62"/>
       <c r="C69" s="8"/>
       <c r="D69" s="2"/>
-      <c r="E69" s="115"/>
-      <c r="F69" s="77"/>
-      <c r="G69" s="77"/>
-      <c r="H69" s="67"/>
-      <c r="J69" s="93"/>
-      <c r="K69" s="99" t="str">
-        <f>IF(M69=1,"OK","ERROR! Ensure Weighting total = 100%")</f>
-        <v>OK</v>
-      </c>
-      <c r="L69" s="94"/>
-      <c r="M69" s="103">
-        <f>SUM(M64:M68)</f>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="N69" s="95"/>
+      <c r="E69" s="109"/>
+      <c r="F69" s="73"/>
+      <c r="G69" s="73"/>
+      <c r="H69" s="63"/>
+      <c r="J69" s="88"/>
+      <c r="K69" s="99"/>
+      <c r="L69" s="89"/>
+      <c r="M69" s="89"/>
+      <c r="N69" s="90"/>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B70" s="66"/>
+      <c r="B70" s="62"/>
       <c r="C70" s="24"/>
       <c r="D70" s="24"/>
-      <c r="E70" s="78"/>
-      <c r="F70" s="78"/>
-      <c r="G70" s="78"/>
-      <c r="H70" s="67"/>
-      <c r="J70" s="93"/>
-      <c r="K70" s="104" t="s">
+      <c r="E70" s="74"/>
+      <c r="F70" s="74"/>
+      <c r="G70" s="74"/>
+      <c r="H70" s="63"/>
+      <c r="J70" s="88"/>
+      <c r="K70" s="98" t="s">
         <v>216</v>
       </c>
-      <c r="L70" s="94"/>
-      <c r="M70" s="94"/>
-      <c r="N70" s="95"/>
+      <c r="L70" s="89"/>
+      <c r="M70" s="89"/>
+      <c r="N70" s="90"/>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B71" s="66"/>
-      <c r="C71" s="82" t="s">
-        <v>208</v>
-      </c>
-      <c r="D71" s="78"/>
-      <c r="E71" s="78"/>
-      <c r="F71" s="78"/>
-      <c r="G71" s="78"/>
-      <c r="H71" s="67"/>
-      <c r="J71" s="93"/>
-      <c r="K71" s="105" t="str">
+      <c r="B71" s="62"/>
+      <c r="C71" s="116" t="s">
+        <v>252</v>
+      </c>
+      <c r="D71" s="76"/>
+      <c r="E71" s="76"/>
+      <c r="F71" s="74"/>
+      <c r="G71" s="74"/>
+      <c r="H71" s="63"/>
+      <c r="J71" s="88"/>
+      <c r="K71" s="99" t="str">
         <f>"          "&amp;M64&amp;" * "&amp;K64&amp;" +"</f>
         <v xml:space="preserve">          0.6 * Median IRI +</v>
       </c>
-      <c r="L71" s="94"/>
-      <c r="M71" s="94"/>
-      <c r="N71" s="95"/>
+      <c r="L71" s="89"/>
+      <c r="M71" s="89"/>
+      <c r="N71" s="90"/>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B72" s="66"/>
-      <c r="C72" s="83" t="s">
+      <c r="B72" s="62"/>
+      <c r="C72" s="72" t="s">
+        <v>253</v>
+      </c>
+      <c r="D72" s="75" t="s">
+        <v>254</v>
+      </c>
+      <c r="E72" s="75" t="s">
+        <v>255</v>
+      </c>
+      <c r="F72" s="74"/>
+      <c r="G72" s="74"/>
+      <c r="H72" s="63"/>
+      <c r="J72" s="88"/>
+      <c r="K72" s="99" t="str">
+        <f>"          "&amp;M65&amp;" * "&amp;K65&amp;" +"</f>
+        <v xml:space="preserve">          0.1 * Minimum IRI  +</v>
+      </c>
+      <c r="L72" s="89"/>
+      <c r="M72" s="89"/>
+      <c r="N72" s="90"/>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B73" s="62"/>
+      <c r="C73" s="117">
+        <v>1</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F73" s="74"/>
+      <c r="G73" s="74"/>
+      <c r="H73" s="63"/>
+      <c r="J73" s="88"/>
+      <c r="K73" s="99" t="str">
+        <f>"          "&amp;M66&amp;" * "&amp;K66&amp;" +"</f>
+        <v xml:space="preserve">          0.2 * Maximum IRI +</v>
+      </c>
+      <c r="L73" s="89"/>
+      <c r="M73" s="89"/>
+      <c r="N73" s="90"/>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B74" s="62"/>
+      <c r="C74" s="117">
+        <v>2</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F74" s="74"/>
+      <c r="G74" s="74"/>
+      <c r="H74" s="63"/>
+      <c r="J74" s="88"/>
+      <c r="K74" s="99" t="str">
+        <f>"          "&amp;M67&amp;" * "&amp;K67&amp;" )"</f>
+        <v xml:space="preserve">          0.1 * Mean IRI )</v>
+      </c>
+      <c r="L74" s="89"/>
+      <c r="M74" s="89"/>
+      <c r="N74" s="90"/>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B75" s="62"/>
+      <c r="C75" s="117">
+        <v>3</v>
+      </c>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="74"/>
+      <c r="G75" s="74"/>
+      <c r="H75" s="63"/>
+      <c r="J75" s="88"/>
+      <c r="K75" s="99"/>
+      <c r="L75" s="89"/>
+      <c r="M75" s="89"/>
+      <c r="N75" s="90"/>
+    </row>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B76" s="62"/>
+      <c r="C76" s="117">
+        <v>4</v>
+      </c>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="74"/>
+      <c r="G76" s="74"/>
+      <c r="H76" s="63"/>
+      <c r="J76" s="88"/>
+      <c r="K76" s="99"/>
+      <c r="L76" s="89"/>
+      <c r="M76" s="89"/>
+      <c r="N76" s="90"/>
+    </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B77" s="62"/>
+      <c r="C77" s="117">
+        <v>5</v>
+      </c>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="74"/>
+      <c r="G77" s="74"/>
+      <c r="H77" s="63"/>
+      <c r="J77" s="88"/>
+      <c r="K77" s="99"/>
+      <c r="L77" s="89"/>
+      <c r="M77" s="89"/>
+      <c r="N77" s="90"/>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B78" s="62"/>
+      <c r="C78" s="117">
+        <v>6</v>
+      </c>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="74"/>
+      <c r="G78" s="74"/>
+      <c r="H78" s="63"/>
+      <c r="J78" s="88"/>
+      <c r="K78" s="99"/>
+      <c r="L78" s="89"/>
+      <c r="M78" s="89"/>
+      <c r="N78" s="90"/>
+    </row>
+    <row r="79" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B79" s="62"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="74"/>
+      <c r="F79" s="74"/>
+      <c r="G79" s="74"/>
+      <c r="H79" s="63"/>
+      <c r="J79" s="88"/>
+      <c r="K79" s="99"/>
+      <c r="L79" s="89"/>
+      <c r="M79" s="89"/>
+      <c r="N79" s="90"/>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B80" s="62"/>
+      <c r="C80" s="77" t="s">
+        <v>208</v>
+      </c>
+      <c r="D80" s="74"/>
+      <c r="E80" s="74"/>
+      <c r="F80" s="74"/>
+      <c r="G80" s="74"/>
+      <c r="H80" s="63"/>
+      <c r="J80" s="88"/>
+      <c r="K80" s="99"/>
+      <c r="L80" s="89"/>
+      <c r="M80" s="89"/>
+      <c r="N80" s="90"/>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B81" s="62"/>
+      <c r="C81" s="78" t="s">
         <v>212</v>
       </c>
-      <c r="D72" s="24"/>
-      <c r="E72" s="78"/>
-      <c r="F72" s="78"/>
-      <c r="G72" s="78"/>
-      <c r="H72" s="67"/>
-      <c r="J72" s="93"/>
-      <c r="K72" s="105" t="str">
-        <f>"          "&amp;M65&amp;" * "&amp;K65&amp;" +"</f>
-        <v xml:space="preserve">          0.1 * Standard deviation of IRI +</v>
-      </c>
-      <c r="L72" s="94"/>
-      <c r="M72" s="94"/>
-      <c r="N72" s="95"/>
-    </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B73" s="66"/>
-      <c r="C73" s="83"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="78"/>
-      <c r="F73" s="78"/>
-      <c r="G73" s="78"/>
-      <c r="H73" s="67"/>
-      <c r="J73" s="93"/>
-      <c r="K73" s="105" t="str">
-        <f>"          "&amp;M66&amp;" * "&amp;K66&amp;" +"</f>
-        <v xml:space="preserve">          0.1 * Minimum IRI  +</v>
-      </c>
-      <c r="L73" s="94"/>
-      <c r="M73" s="94"/>
-      <c r="N73" s="95"/>
-    </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B74" s="66"/>
-      <c r="C74" s="76" t="s">
+      <c r="D81" s="24"/>
+      <c r="E81" s="74"/>
+      <c r="F81" s="74"/>
+      <c r="G81" s="74"/>
+      <c r="H81" s="63"/>
+      <c r="J81" s="88"/>
+      <c r="K81" s="99"/>
+      <c r="L81" s="89"/>
+      <c r="M81" s="89"/>
+      <c r="N81" s="90"/>
+    </row>
+    <row r="82" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B82" s="62"/>
+      <c r="C82" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="D74" s="76"/>
-      <c r="E74" s="79" t="s">
+      <c r="D82" s="72"/>
+      <c r="E82" s="75" t="s">
         <v>206</v>
       </c>
-      <c r="F74" s="78"/>
-      <c r="G74" s="78"/>
-      <c r="H74" s="67"/>
-      <c r="J74" s="93"/>
-      <c r="K74" s="105" t="str">
-        <f>"          "&amp;M67&amp;" * "&amp;K67&amp;" +"</f>
-        <v xml:space="preserve">          0.1 * Maximum IRI +</v>
-      </c>
-      <c r="L74" s="94"/>
-      <c r="M74" s="94"/>
-      <c r="N74" s="95"/>
-    </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B75" s="66"/>
-      <c r="C75" s="8" t="s">
+      <c r="F82" s="74"/>
+      <c r="G82" s="74"/>
+      <c r="H82" s="63"/>
+      <c r="J82" s="88"/>
+      <c r="K82" s="99"/>
+      <c r="L82" s="89"/>
+      <c r="M82" s="89"/>
+      <c r="N82" s="90"/>
+    </row>
+    <row r="83" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B83" s="62"/>
+      <c r="C83" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="D75" s="2"/>
-      <c r="E75" s="101">
+      <c r="D83" s="2"/>
+      <c r="E83" s="95">
         <v>0.5</v>
       </c>
-      <c r="F75" s="78"/>
-      <c r="G75" s="78"/>
-      <c r="H75" s="67"/>
-      <c r="J75" s="93"/>
-      <c r="K75" s="105" t="str">
-        <f>"          "&amp;M68&amp;" * "&amp;K68&amp;" )"</f>
-        <v xml:space="preserve">          0.1 * Mean IRI )</v>
-      </c>
-      <c r="L75" s="94"/>
-      <c r="M75" s="94"/>
-      <c r="N75" s="95"/>
-    </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B76" s="66"/>
-      <c r="C76" s="8" t="s">
+      <c r="F83" s="74"/>
+      <c r="G83" s="74"/>
+      <c r="H83" s="63"/>
+      <c r="J83" s="88"/>
+      <c r="K83" s="99"/>
+      <c r="L83" s="89"/>
+      <c r="M83" s="89"/>
+      <c r="N83" s="90"/>
+    </row>
+    <row r="84" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B84" s="62"/>
+      <c r="C84" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="D76" s="2"/>
-      <c r="E76" s="101">
+      <c r="D84" s="2"/>
+      <c r="E84" s="95">
         <v>0.25</v>
       </c>
-      <c r="F76" s="78"/>
-      <c r="G76" s="78"/>
-      <c r="H76" s="67"/>
-      <c r="J76" s="93"/>
-      <c r="K76" s="100"/>
-      <c r="L76" s="94"/>
-      <c r="M76" s="94"/>
-      <c r="N76" s="95"/>
-    </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B77" s="66"/>
-      <c r="C77" s="84" t="s">
+      <c r="F84" s="74"/>
+      <c r="G84" s="74"/>
+      <c r="H84" s="63"/>
+      <c r="J84" s="88"/>
+      <c r="K84" s="99"/>
+      <c r="L84" s="89"/>
+      <c r="M84" s="89"/>
+      <c r="N84" s="90"/>
+    </row>
+    <row r="85" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B85" s="62"/>
+      <c r="C85" s="79" t="s">
         <v>211</v>
       </c>
-      <c r="D77" s="85" t="str">
-        <f>"Length (km) * ("&amp;E75&amp;" + "&amp;E76&amp;" * IRI)"</f>
+      <c r="D85" s="80" t="str">
+        <f>"Length (km) * ("&amp;E83&amp;" + "&amp;E84&amp;" * IRI)"</f>
         <v>Length (km) * (0.5 + 0.25 * IRI)</v>
       </c>
-      <c r="E77" s="86"/>
-      <c r="F77" s="78"/>
-      <c r="G77" s="78"/>
-      <c r="H77" s="67"/>
-      <c r="J77" s="93"/>
-      <c r="K77" s="94"/>
-      <c r="L77" s="94"/>
-      <c r="M77" s="94"/>
-      <c r="N77" s="95"/>
-    </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B78" s="66"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="78"/>
-      <c r="F78" s="78"/>
-      <c r="G78" s="78"/>
-      <c r="H78" s="67"/>
-      <c r="J78" s="93"/>
-      <c r="K78" s="94"/>
-      <c r="L78" s="94"/>
-      <c r="M78" s="94"/>
-      <c r="N78" s="95"/>
-    </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B79" s="66"/>
-      <c r="C79" s="75" t="s">
+      <c r="E85" s="81"/>
+      <c r="F85" s="74"/>
+      <c r="G85" s="74"/>
+      <c r="H85" s="63"/>
+      <c r="J85" s="88"/>
+      <c r="K85" s="99"/>
+      <c r="L85" s="89"/>
+      <c r="M85" s="89"/>
+      <c r="N85" s="90"/>
+    </row>
+    <row r="86" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B86" s="62"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="74"/>
+      <c r="F86" s="74"/>
+      <c r="G86" s="74"/>
+      <c r="H86" s="63"/>
+      <c r="J86" s="88"/>
+      <c r="K86" s="89"/>
+      <c r="L86" s="89"/>
+      <c r="M86" s="89"/>
+      <c r="N86" s="90"/>
+    </row>
+    <row r="87" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B87" s="62"/>
+      <c r="C87" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="D79" s="24"/>
-      <c r="E79" s="78"/>
-      <c r="F79" s="78"/>
-      <c r="G79" s="78"/>
-      <c r="H79" s="67"/>
-      <c r="J79" s="93"/>
-      <c r="K79" s="94"/>
-      <c r="L79" s="94"/>
-      <c r="M79" s="94"/>
-      <c r="N79" s="95"/>
-    </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B80" s="66"/>
-      <c r="C80" s="76" t="s">
+      <c r="D87" s="24"/>
+      <c r="E87" s="74"/>
+      <c r="F87" s="74"/>
+      <c r="G87" s="74"/>
+      <c r="H87" s="63"/>
+      <c r="J87" s="88"/>
+      <c r="K87" s="89"/>
+      <c r="L87" s="89"/>
+      <c r="M87" s="89"/>
+      <c r="N87" s="90"/>
+    </row>
+    <row r="88" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B88" s="62"/>
+      <c r="C88" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="D80" s="79" t="s">
+      <c r="D88" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="E80" s="78"/>
-      <c r="F80" s="78"/>
-      <c r="G80" s="78"/>
-      <c r="H80" s="67"/>
-      <c r="J80" s="93"/>
-      <c r="K80" s="94"/>
-      <c r="L80" s="94"/>
-      <c r="M80" s="94"/>
-      <c r="N80" s="95"/>
-    </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B81" s="66"/>
-      <c r="C81" s="8" t="s">
+      <c r="E88" s="74"/>
+      <c r="F88" s="74"/>
+      <c r="G88" s="74"/>
+      <c r="H88" s="63"/>
+      <c r="J88" s="88"/>
+      <c r="K88" s="89"/>
+      <c r="L88" s="89"/>
+      <c r="M88" s="89"/>
+      <c r="N88" s="90"/>
+    </row>
+    <row r="89" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B89" s="62"/>
+      <c r="C89" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D89" s="2">
         <v>0.8</v>
       </c>
-      <c r="E81" s="78"/>
-      <c r="F81" s="78"/>
-      <c r="G81" s="78"/>
-      <c r="H81" s="67"/>
-      <c r="J81" s="93"/>
-      <c r="K81" s="94"/>
-      <c r="L81" s="94"/>
-      <c r="M81" s="94"/>
-      <c r="N81" s="95"/>
-    </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B82" s="66"/>
-      <c r="C82" s="8" t="s">
+      <c r="E89" s="74"/>
+      <c r="F89" s="74"/>
+      <c r="G89" s="74"/>
+      <c r="H89" s="63"/>
+      <c r="J89" s="88"/>
+      <c r="K89" s="89"/>
+      <c r="L89" s="89"/>
+      <c r="M89" s="89"/>
+      <c r="N89" s="90"/>
+    </row>
+    <row r="90" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B90" s="62"/>
+      <c r="C90" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D90" s="2">
         <v>0.2</v>
       </c>
-      <c r="E82" s="78"/>
-      <c r="F82" s="78"/>
-      <c r="G82" s="78"/>
-      <c r="H82" s="67"/>
-      <c r="J82" s="93"/>
-      <c r="K82" s="94"/>
-      <c r="L82" s="94"/>
-      <c r="M82" s="94"/>
-      <c r="N82" s="95"/>
-    </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B83" s="66"/>
-      <c r="C83" s="78"/>
-      <c r="D83" s="102">
-        <f>SUM(D81:D82)</f>
+      <c r="E90" s="74"/>
+      <c r="F90" s="74"/>
+      <c r="G90" s="74"/>
+      <c r="H90" s="63"/>
+      <c r="J90" s="88"/>
+      <c r="K90" s="89"/>
+      <c r="L90" s="89"/>
+      <c r="M90" s="89"/>
+      <c r="N90" s="90"/>
+    </row>
+    <row r="91" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B91" s="62"/>
+      <c r="C91" s="74"/>
+      <c r="D91" s="96">
+        <f>SUM(D89:D90)</f>
         <v>1</v>
       </c>
-      <c r="E83" s="78"/>
-      <c r="F83" s="78"/>
-      <c r="G83" s="78"/>
-      <c r="H83" s="67"/>
-      <c r="J83" s="93"/>
-      <c r="K83" s="94"/>
-      <c r="L83" s="94"/>
-      <c r="M83" s="94"/>
-      <c r="N83" s="95"/>
-    </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B84" s="68"/>
-      <c r="C84" s="69"/>
-      <c r="D84" s="69"/>
-      <c r="E84" s="69"/>
-      <c r="F84" s="69"/>
-      <c r="G84" s="69"/>
-      <c r="H84" s="70"/>
-      <c r="J84" s="96"/>
-      <c r="K84" s="97"/>
-      <c r="L84" s="97"/>
-      <c r="M84" s="97"/>
-      <c r="N84" s="98"/>
+      <c r="E91" s="74"/>
+      <c r="F91" s="74"/>
+      <c r="G91" s="74"/>
+      <c r="H91" s="63"/>
+      <c r="J91" s="88"/>
+      <c r="K91" s="89"/>
+      <c r="L91" s="89"/>
+      <c r="M91" s="89"/>
+      <c r="N91" s="90"/>
+    </row>
+    <row r="92" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B92" s="64"/>
+      <c r="C92" s="65"/>
+      <c r="D92" s="65"/>
+      <c r="E92" s="65"/>
+      <c r="F92" s="65"/>
+      <c r="G92" s="65"/>
+      <c r="H92" s="66"/>
+      <c r="J92" s="91"/>
+      <c r="K92" s="92"/>
+      <c r="L92" s="92"/>
+      <c r="M92" s="92"/>
+      <c r="N92" s="93"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L16">
@@ -5328,12 +5559,12 @@
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
+  <conditionalFormatting sqref="K68">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E36:E49">
       <formula1>"Relative,Absolute"</formula1>
     </dataValidation>
@@ -5343,6 +5574,12 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G67:G69">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D73:D78">
+      <formula1>$C$61:$C$64</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E73:E78">
+      <formula1>$C$67:$C$70</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5350,7 +5587,7 @@
   <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Ref!$A$3:$A$38</xm:f>
@@ -5385,17 +5622,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="61">
+      <c r="B2" s="57">
         <f>+Input!M10</f>
         <v>0.2</v>
       </c>
@@ -5404,7 +5641,7 @@
       <c r="A3" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="61">
+      <c r="B3" s="57">
         <f>+Input!M11</f>
         <v>0.2</v>
       </c>
@@ -5413,7 +5650,7 @@
       <c r="A4" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="61">
+      <c r="B4" s="57">
         <f>+Input!M12</f>
         <v>0.25</v>
       </c>
@@ -5422,7 +5659,7 @@
       <c r="A5" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="61">
+      <c r="B5" s="57">
         <f>+Input!M13</f>
         <v>0.25</v>
       </c>
@@ -5431,7 +5668,7 @@
       <c r="A6" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="61">
+      <c r="B6" s="57">
         <f>+Input!M14</f>
         <v>0.1</v>
       </c>
@@ -5443,10 +5680,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5459,7 +5696,7 @@
         <v>188</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>126</v>
@@ -5467,24 +5704,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="106">
+      <c r="C2" s="100">
         <f>+Input!M64</f>
         <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B3" t="s">
         <v>217</v>
       </c>
-      <c r="C3" s="106">
+      <c r="C3" s="100">
         <f>+Input!M65</f>
         <v>0.1</v>
       </c>
@@ -5496,9 +5733,9 @@
       <c r="B4" t="s">
         <v>218</v>
       </c>
-      <c r="C4" s="106">
+      <c r="C4" s="100">
         <f>+Input!M66</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -5508,20 +5745,8 @@
       <c r="B5" t="s">
         <v>219</v>
       </c>
-      <c r="C5" s="106">
+      <c r="C5" s="100">
         <f>+Input!M67</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C6" s="106">
-        <f>+Input!M68</f>
         <v>0.1</v>
       </c>
     </row>
@@ -5534,647 +5759,649 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.5546875" customWidth="1"/>
-    <col min="4" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" style="111" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" style="111" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" style="111" customWidth="1"/>
+    <col min="4" max="5" width="10.33203125" style="111" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="111" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="111"/>
+    <col min="9" max="9" width="51.6640625" style="111" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="111"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="110" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="110" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="110" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="110" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="110" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="110" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="110" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="110" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="110" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="111" t="s">
         <v>157</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="111" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="51">
+      <c r="D2" s="113">
         <v>1</v>
       </c>
-      <c r="E2" s="51">
+      <c r="E2" s="113">
         <v>100</v>
       </c>
-      <c r="F2" s="52">
+      <c r="F2" s="114">
         <f>+Input!D36</f>
         <v>0.03</v>
       </c>
-      <c r="G2" s="52" t="str">
+      <c r="G2" s="114" t="str">
         <f>Input!E36</f>
         <v>Relative</v>
       </c>
-      <c r="H2" s="53">
+      <c r="H2" s="115">
         <f>+Input!F36</f>
         <v>50</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="111" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="111" t="s">
         <v>158</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="111" t="s">
         <v>158</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="112" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="51">
+      <c r="D3" s="113">
         <v>1</v>
       </c>
-      <c r="E3" s="51">
+      <c r="E3" s="113">
         <v>100</v>
       </c>
-      <c r="F3" s="52">
+      <c r="F3" s="114">
         <f>+Input!D37</f>
         <v>0.01</v>
       </c>
-      <c r="G3" s="52" t="str">
+      <c r="G3" s="114" t="str">
         <f>Input!E37</f>
         <v>Relative</v>
       </c>
-      <c r="H3" s="53">
+      <c r="H3" s="115">
         <f>+Input!F37</f>
         <v>50</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="111" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="111" t="s">
         <v>159</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="111" t="s">
         <v>159</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="111" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="51">
+      <c r="D4" s="113">
         <v>0</v>
       </c>
-      <c r="E4" s="51">
+      <c r="E4" s="113">
         <v>10</v>
       </c>
-      <c r="F4" s="52">
+      <c r="F4" s="114">
         <f>+Input!D38</f>
         <v>0.15</v>
       </c>
-      <c r="G4" s="52" t="str">
+      <c r="G4" s="114" t="str">
         <f>Input!E38</f>
         <v>Relative</v>
       </c>
-      <c r="H4" s="53">
+      <c r="H4" s="115">
         <f>+Input!F38</f>
         <v>0.5</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="111" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="111" t="s">
         <v>160</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="111" t="s">
         <v>160</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="111" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="113">
         <v>0</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="113">
         <v>10</v>
       </c>
-      <c r="F5" s="52">
+      <c r="F5" s="114">
         <f>+Input!D39</f>
         <v>0.1</v>
       </c>
-      <c r="G5" s="52" t="str">
+      <c r="G5" s="114" t="str">
         <f>Input!E39</f>
         <v>Relative</v>
       </c>
-      <c r="H5" s="53">
+      <c r="H5" s="115">
         <f>+Input!F39</f>
         <v>0.5</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="111" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="111" t="s">
         <v>161</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="111" t="s">
         <v>161</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="111" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="113">
         <v>0</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="113">
         <v>10</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="114">
         <f>+Input!D40</f>
         <v>0.05</v>
       </c>
-      <c r="G6" s="52" t="str">
+      <c r="G6" s="114" t="str">
         <f>Input!E40</f>
         <v>Relative</v>
       </c>
-      <c r="H6" s="53">
+      <c r="H6" s="115">
         <f>+Input!F40</f>
         <v>0.5</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="111" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="111" t="s">
         <v>162</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="111" t="s">
         <v>162</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="111" t="s">
         <v>154</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="113">
         <v>0</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="113">
         <v>10</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="114">
         <f>+Input!D41</f>
         <v>0.1</v>
       </c>
-      <c r="G7" s="52" t="str">
+      <c r="G7" s="114" t="str">
         <f>Input!E41</f>
         <v>Relative</v>
       </c>
-      <c r="H7" s="53">
+      <c r="H7" s="115">
         <f>+Input!F41</f>
         <v>0.5</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="111" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="111" t="s">
         <v>163</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="111" t="s">
         <v>163</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="111" t="s">
         <v>155</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="113">
         <v>0</v>
       </c>
-      <c r="E8" s="51">
+      <c r="E8" s="113">
         <v>10</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="114">
         <f>+Input!D42</f>
         <v>0.05</v>
       </c>
-      <c r="G8" s="52" t="str">
+      <c r="G8" s="114" t="str">
         <f>Input!E42</f>
         <v>Relative</v>
       </c>
-      <c r="H8" s="53">
+      <c r="H8" s="115">
         <f>+Input!F42</f>
         <v>0.5</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="111" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="111" t="s">
         <v>164</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="111" t="s">
         <v>164</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="111" t="s">
         <v>156</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="113">
         <v>0</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="113">
         <v>10</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="114">
         <f>+Input!D43</f>
         <v>0.03</v>
       </c>
-      <c r="G9" s="52" t="str">
+      <c r="G9" s="114" t="str">
         <f>Input!E43</f>
         <v>Relative</v>
       </c>
-      <c r="H9" s="53">
+      <c r="H9" s="115">
         <f>+Input!F43</f>
         <v>0.5</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="111" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="111" t="s">
         <v>165</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="111" t="s">
         <v>165</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="111" t="s">
         <v>148</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="113">
         <v>0</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E10" s="113">
         <v>10</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="114">
         <f>+Input!D44</f>
         <v>0.1</v>
       </c>
-      <c r="G10" s="52" t="str">
+      <c r="G10" s="114" t="str">
         <f>Input!E44</f>
         <v>Relative</v>
       </c>
-      <c r="H10" s="53">
+      <c r="H10" s="115">
         <f>+Input!F44</f>
         <v>0.5</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="111" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="111" t="s">
         <v>166</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="111" t="s">
         <v>166</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="111" t="s">
         <v>149</v>
       </c>
-      <c r="D11" s="51">
+      <c r="D11" s="113">
         <v>0</v>
       </c>
-      <c r="E11" s="51">
+      <c r="E11" s="113">
         <v>10</v>
       </c>
-      <c r="F11" s="52">
+      <c r="F11" s="114">
         <f>+Input!D45</f>
         <v>0.05</v>
       </c>
-      <c r="G11" s="52" t="str">
+      <c r="G11" s="114" t="str">
         <f>Input!E45</f>
         <v>Relative</v>
       </c>
-      <c r="H11" s="53">
+      <c r="H11" s="115">
         <f>+Input!F45</f>
         <v>0.5</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="111" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="111" t="s">
         <v>167</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="111" t="s">
         <v>167</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="111" t="s">
         <v>150</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="113">
         <v>0</v>
       </c>
-      <c r="E12" s="51">
+      <c r="E12" s="113">
         <v>10</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F12" s="114">
         <f>+Input!D46</f>
         <v>0.03</v>
       </c>
-      <c r="G12" s="52" t="str">
+      <c r="G12" s="114" t="str">
         <f>Input!E46</f>
         <v>Relative</v>
       </c>
-      <c r="H12" s="53">
+      <c r="H12" s="115">
         <f>+Input!F46</f>
         <v>0.5</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="111" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="111" t="s">
         <v>168</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="111" t="s">
         <v>168</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="111" t="s">
         <v>131</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="113">
         <v>1</v>
       </c>
-      <c r="E13" s="51">
+      <c r="E13" s="113">
         <v>100</v>
       </c>
-      <c r="F13" s="52">
+      <c r="F13" s="114">
         <f>+Input!D47</f>
         <v>0.03</v>
       </c>
-      <c r="G13" s="52" t="str">
+      <c r="G13" s="114" t="str">
         <f>Input!E47</f>
         <v>Relative</v>
       </c>
-      <c r="H13" s="53">
+      <c r="H13" s="115">
         <f>+Input!F47</f>
         <v>30</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="111" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="111" t="s">
         <v>169</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="111" t="s">
         <v>169</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="111" t="s">
         <v>132</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="113">
         <v>1</v>
       </c>
-      <c r="E14" s="51">
+      <c r="E14" s="113">
         <v>100</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="114">
         <f>+Input!D48</f>
         <v>0.02</v>
       </c>
-      <c r="G14" s="52" t="str">
+      <c r="G14" s="114" t="str">
         <f>Input!E48</f>
         <v>Relative</v>
       </c>
-      <c r="H14" s="53">
+      <c r="H14" s="115">
         <f>+Input!F48</f>
         <v>30</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="111" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="111" t="s">
         <v>170</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="111" t="s">
         <v>170</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="111" t="s">
         <v>133</v>
       </c>
-      <c r="D15" s="51">
+      <c r="D15" s="113">
         <v>1</v>
       </c>
-      <c r="E15" s="51">
+      <c r="E15" s="113">
         <v>100</v>
       </c>
-      <c r="F15" s="52">
+      <c r="F15" s="114">
         <f>+Input!D49</f>
         <v>0.01</v>
       </c>
-      <c r="G15" s="52" t="str">
+      <c r="G15" s="114" t="str">
         <f>Input!E49</f>
         <v>Relative</v>
       </c>
-      <c r="H15" s="53">
+      <c r="H15" s="115">
         <f>+Input!F49</f>
         <v>30</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="111" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="111" t="s">
         <v>171</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="111" t="s">
         <v>171</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="112" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="51">
+      <c r="D16" s="113">
         <v>1</v>
       </c>
-      <c r="E16" s="51">
+      <c r="E16" s="113">
         <v>500</v>
       </c>
-      <c r="F16" s="52">
+      <c r="F16" s="114">
         <f>+Input!D50</f>
         <v>0.06</v>
       </c>
-      <c r="G16" s="52" t="str">
+      <c r="G16" s="114" t="str">
         <f>Input!E50</f>
         <v>Relative</v>
       </c>
-      <c r="H16" s="53">
+      <c r="H16" s="115">
         <f>+Input!F50</f>
         <v>0</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="111" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="111" t="s">
         <v>172</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="111" t="s">
         <v>172</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="111" t="s">
         <v>124</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="113">
         <v>1</v>
       </c>
-      <c r="E17" s="51">
+      <c r="E17" s="113">
         <v>500</v>
       </c>
-      <c r="F17" s="52">
+      <c r="F17" s="114">
         <f>+Input!D51</f>
         <v>0.04</v>
       </c>
-      <c r="G17" s="52" t="str">
+      <c r="G17" s="114" t="str">
         <f>Input!E51</f>
         <v>Relative</v>
       </c>
-      <c r="H17" s="53">
+      <c r="H17" s="115">
         <f>+Input!F51</f>
         <v>0</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="111" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="111" t="s">
         <v>173</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="111" t="s">
         <v>173</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="111" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="51">
+      <c r="D18" s="113">
         <v>1</v>
       </c>
-      <c r="E18" s="51">
+      <c r="E18" s="113">
         <v>500</v>
       </c>
-      <c r="F18" s="52">
+      <c r="F18" s="114">
         <f>+Input!D52</f>
         <v>0.02</v>
       </c>
-      <c r="G18" s="52" t="str">
+      <c r="G18" s="114" t="str">
         <f>Input!E52</f>
         <v>Relative</v>
       </c>
-      <c r="H18" s="53">
+      <c r="H18" s="115">
         <f>+Input!F52</f>
         <v>0</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="111" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="111" t="s">
         <v>174</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="111" t="s">
         <v>174</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="111" t="s">
         <v>128</v>
       </c>
-      <c r="D19" s="51">
+      <c r="D19" s="113">
         <v>0</v>
       </c>
-      <c r="E19" s="51">
+      <c r="E19" s="113">
         <v>1</v>
       </c>
-      <c r="F19" s="52">
+      <c r="F19" s="114">
         <f>+Input!D53</f>
         <v>0.02</v>
       </c>
-      <c r="G19" s="52" t="str">
+      <c r="G19" s="114" t="str">
         <f>Input!E53</f>
         <v>Relative</v>
       </c>
-      <c r="H19" s="53">
+      <c r="H19" s="115">
         <f>+Input!F53</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="111" t="s">
         <v>192</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="111" t="s">
         <v>192</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="111" t="s">
         <v>193</v>
       </c>
-      <c r="D20" s="51">
+      <c r="D20" s="113">
         <v>0</v>
       </c>
-      <c r="E20" s="51">
+      <c r="E20" s="113">
         <v>5</v>
       </c>
-      <c r="F20" s="52">
+      <c r="F20" s="114">
         <f>+Input!D54</f>
         <v>0.1</v>
       </c>
-      <c r="G20" s="52" t="str">
+      <c r="G20" s="114" t="str">
         <f>Input!E54</f>
         <v>Relative</v>
       </c>
-      <c r="H20" s="53">
+      <c r="H20" s="115">
         <f>+Input!F54</f>
         <v>0</v>
       </c>
@@ -6221,7 +6448,7 @@
         <f t="shared" ref="B2:B11" si="0">"__"&amp;LEFT(E2,8)</f>
         <v>__hhsize_c</v>
       </c>
-      <c r="C2" s="61">
+      <c r="C2" s="57">
         <f>Input!D10</f>
         <v>0.05</v>
       </c>
@@ -6242,7 +6469,7 @@
         <f t="shared" si="0"/>
         <v>__roof_1cm</v>
       </c>
-      <c r="C3" s="61">
+      <c r="C3" s="57">
         <f>Input!D11</f>
         <v>0.05</v>
       </c>
@@ -6263,7 +6490,7 @@
         <f t="shared" si="0"/>
         <v>__water_1c</v>
       </c>
-      <c r="C4" s="61">
+      <c r="C4" s="57">
         <f>Input!D12</f>
         <v>0.2</v>
       </c>
@@ -6284,7 +6511,7 @@
         <f t="shared" si="0"/>
         <v>__toilet_1</v>
       </c>
-      <c r="C5" s="61">
+      <c r="C5" s="57">
         <f>Input!D13</f>
         <v>0.1</v>
       </c>
@@ -6305,7 +6532,7 @@
         <f t="shared" si="0"/>
         <v>__edchd_4c</v>
       </c>
-      <c r="C6" s="61">
+      <c r="C6" s="57">
         <f>Input!D14</f>
         <v>0.1</v>
       </c>
@@ -6326,7 +6553,7 @@
         <f t="shared" si="0"/>
         <v>__ethnic_c</v>
       </c>
-      <c r="C7" s="61">
+      <c r="C7" s="57">
         <f>Input!D15</f>
         <v>0.05</v>
       </c>
@@ -6347,7 +6574,7 @@
         <f t="shared" si="0"/>
         <v>__pelderly</v>
       </c>
-      <c r="C8" s="61">
+      <c r="C8" s="57">
         <f>Input!D16</f>
         <v>0.05</v>
       </c>
@@ -6368,7 +6595,7 @@
         <f t="shared" si="0"/>
         <v>__avg_fgt1</v>
       </c>
-      <c r="C9" s="61">
+      <c r="C9" s="57">
         <f>Input!D17</f>
         <v>0.1</v>
       </c>
@@ -6389,7 +6616,7 @@
         <f t="shared" si="0"/>
         <v>__avg_gini</v>
       </c>
-      <c r="C10" s="61">
+      <c r="C10" s="57">
         <f>Input!D18</f>
         <v>0.1</v>
       </c>
@@ -6410,7 +6637,7 @@
         <f t="shared" si="0"/>
         <v>__mean</v>
       </c>
-      <c r="C11" s="61">
+      <c r="C11" s="57">
         <f>Input!D19</f>
         <v>0.2</v>
       </c>
@@ -6430,10 +6657,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6445,56 +6672,66 @@
     <col min="13" max="13" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="113" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="107" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="101" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" s="102" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1" s="102" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="102" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" s="103" t="s">
+        <v>239</v>
+      </c>
+      <c r="G1" s="104" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="107" t="s">
-        <v>239</v>
-      </c>
-      <c r="C1" s="108" t="s">
-        <v>244</v>
-      </c>
-      <c r="D1" s="108" t="s">
+      <c r="H1" s="104" t="s">
         <v>240</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="I1" s="104" t="s">
+        <v>248</v>
+      </c>
+      <c r="J1" s="104" t="s">
+        <v>247</v>
+      </c>
+      <c r="K1" s="104" t="s">
+        <v>245</v>
+      </c>
+      <c r="L1" s="105" t="s">
+        <v>233</v>
+      </c>
+      <c r="M1" s="105" t="s">
+        <v>231</v>
+      </c>
+      <c r="N1" s="105" t="s">
+        <v>232</v>
+      </c>
+      <c r="O1" s="105" t="s">
         <v>243</v>
       </c>
-      <c r="F1" s="109" t="s">
-        <v>241</v>
-      </c>
-      <c r="G1" s="110" t="s">
-        <v>248</v>
-      </c>
-      <c r="H1" s="110" t="s">
-        <v>242</v>
-      </c>
-      <c r="I1" s="110" t="s">
-        <v>250</v>
-      </c>
-      <c r="J1" s="110" t="s">
-        <v>249</v>
-      </c>
-      <c r="K1" s="110" t="s">
-        <v>247</v>
-      </c>
-      <c r="L1" s="111" t="s">
-        <v>235</v>
-      </c>
-      <c r="M1" s="111" t="s">
-        <v>233</v>
-      </c>
-      <c r="N1" s="111" t="s">
-        <v>234</v>
-      </c>
-      <c r="O1" s="111" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="105" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q1" s="105" t="s">
+        <v>257</v>
+      </c>
+      <c r="R1" s="105" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6510,8 +6747,8 @@
         <f>+Input!E61</f>
         <v>0</v>
       </c>
-      <c r="E2" s="112" t="s">
-        <v>237</v>
+      <c r="E2" s="106" t="s">
+        <v>235</v>
       </c>
       <c r="F2" t="str">
         <f>+Input!C67</f>
@@ -6529,31 +6766,43 @@
         <f>+Input!F67</f>
         <v>50</v>
       </c>
-      <c r="J2" s="114">
+      <c r="J2" s="108">
         <f>Input!G67</f>
         <v>1</v>
       </c>
-      <c r="K2" s="112" t="s">
-        <v>237</v>
-      </c>
-      <c r="L2" s="61">
-        <f>+Input!E75</f>
+      <c r="K2" s="106" t="s">
+        <v>235</v>
+      </c>
+      <c r="L2" s="57">
+        <f>+Input!E83</f>
         <v>0.5</v>
       </c>
-      <c r="M2" s="61">
-        <f>+Input!E76</f>
+      <c r="M2" s="57">
+        <f>+Input!E84</f>
         <v>0.25</v>
       </c>
-      <c r="N2" s="106">
-        <f>+Input!D81</f>
+      <c r="N2" s="100">
+        <f>+Input!D89</f>
         <v>0.8</v>
       </c>
-      <c r="O2" s="106">
-        <f>+Input!D82</f>
+      <c r="O2" s="100">
+        <f>+Input!D90</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="118">
+        <f>Input!C73</f>
+        <v>1</v>
+      </c>
+      <c r="Q2" s="118" t="str">
+        <f>Input!D73</f>
+        <v>adm_centroids</v>
+      </c>
+      <c r="R2" s="118" t="str">
+        <f>Input!E73</f>
+        <v>adm_centroids</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6569,7 +6818,7 @@
         <f>+Input!E62</f>
         <v>0</v>
       </c>
-      <c r="E3" s="112"/>
+      <c r="E3" s="106"/>
       <c r="F3" t="str">
         <f>+Input!C68</f>
         <v>Hosptials</v>
@@ -6586,15 +6835,27 @@
         <f>+Input!F68</f>
         <v>3</v>
       </c>
-      <c r="J3" s="114">
+      <c r="J3" s="108">
         <f>Input!G68</f>
         <v>5</v>
       </c>
-      <c r="K3" s="112" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K3" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="P3" s="118">
+        <f>Input!C74</f>
+        <v>2</v>
+      </c>
+      <c r="Q3" s="118" t="str">
+        <f>Input!D74</f>
+        <v>adm_centroids</v>
+      </c>
+      <c r="R3" s="118" t="str">
+        <f>Input!E74</f>
+        <v>Hosptials</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6610,7 +6871,7 @@
         <f>+Input!E63</f>
         <v>0</v>
       </c>
-      <c r="E4" s="112"/>
+      <c r="E4" s="106"/>
       <c r="F4">
         <f>+Input!C69</f>
         <v>0</v>
@@ -6627,20 +6888,79 @@
         <f>+Input!F69</f>
         <v>0</v>
       </c>
-      <c r="J4" s="114">
+      <c r="J4" s="108">
         <f>Input!G69</f>
         <v>0</v>
       </c>
-      <c r="K4" s="112"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K4" s="106"/>
+      <c r="P4" s="118">
+        <f>Input!C75</f>
+        <v>3</v>
+      </c>
+      <c r="Q4" s="118">
+        <f>Input!D75</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="118">
+        <f>Input!E75</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="L5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+      <c r="P5" s="118">
+        <f>Input!C76</f>
+        <v>4</v>
+      </c>
+      <c r="Q5" s="118">
+        <f>Input!D76</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="118">
+        <f>Input!E76</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
       <c r="L6" t="s">
-        <v>238</v>
+        <v>236</v>
+      </c>
+      <c r="P6" s="118">
+        <f>Input!C77</f>
+        <v>5</v>
+      </c>
+      <c r="Q6" s="118">
+        <f>Input!D77</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="118">
+        <f>Input!E77</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="P7" s="118">
+        <f>Input!C78</f>
+        <v>6</v>
+      </c>
+      <c r="Q7" s="118">
+        <f>Input!D78</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="118">
+        <f>Input!E78</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6664,21 +6984,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="59" t="s">
         <v>188</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="59" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C2">

</xml_diff>